<commit_message>
correção do sem técnico // resumo iniciado
</commit_message>
<xml_diff>
--- a/inputs/0 - Expansão/0 - Monitoramento Form 1, 2 e 3.xlsx
+++ b/inputs/0 - Expansão/0 - Monitoramento Form 1, 2 e 3.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29128"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_A8456F674786C56506D9E2B3A45DDC74AC4C4116" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62FD60A5-4874-4B72-A042-11EE125B1EC8}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_A8456F674736C33B12D9FCFEBCDDC741BC897632" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1543FF62-3D14-41E4-B2E6-DDA9BEE9B5E2}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1727,19 +1727,19 @@
       </c>
       <c r="D3" s="17">
         <f ca="1">COUNTIF(INDIRECT("'Form 2 - UVR'!E2:E100"),"Atrasado")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="18">
         <f ca="1">D3/SUM($B3,$D3,$F3)</f>
-        <v>0</v>
+        <v>1.9230769230769232E-2</v>
       </c>
       <c r="F3" s="17">
         <f ca="1">COUNTIF(INDIRECT("'Form 2 - UVR'!E2:E100"),"Sem Técnico")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3" s="18">
         <f ca="1">F3/SUM($B3,$D3,$F3)</f>
-        <v>3.8461538461538464E-2</v>
+        <v>1.9230769230769232E-2</v>
       </c>
       <c r="H3" s="19">
         <f ca="1">SUM(B3,D3,F3)</f>
@@ -1793,19 +1793,19 @@
       </c>
       <c r="D5" s="19">
         <f ca="1">SUM(D2:D4)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E5" s="18">
         <f ca="1">D5/SUM($B5,$D5,$F5)</f>
-        <v>1.2345679012345678E-2</v>
+        <v>1.8518518518518517E-2</v>
       </c>
       <c r="F5" s="19">
         <f ca="1">SUM(F2:F4)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G5" s="18">
         <f ca="1">F5/SUM($B5,$D5,$F5)</f>
-        <v>2.4691358024691357E-2</v>
+        <v>1.8518518518518517E-2</v>
       </c>
       <c r="H5" s="19">
         <f ca="1">SUM(B5,D5,F5)</f>
@@ -1822,7 +1822,7 @@
   <dimension ref="A1:K58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" topLeftCell="D50" activePane="topRight" state="frozen"/>
+      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
@@ -3636,8 +3636,8 @@
   <dimension ref="A1:K58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" topLeftCell="D41" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G50" sqref="G50"/>
+      <pane xSplit="3" topLeftCell="D16" activePane="topRight" state="frozen"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4228,8 +4228,8 @@
         <f>IFERROR(IF(INDEX('Form 1 - Município'!D2:D500, MATCH(B19&amp;C19, INDEX('Form 1 - Município'!B2:B500&amp;'Form 1 - Município'!C2:C500, 0), 0))="", "", INDEX('Form 1 - Município'!D2:D500, MATCH(B19&amp;C19, INDEX('Form 1 - Município'!B2:B500&amp;'Form 1 - Município'!C2:C500, 0), 0))), "")</f>
         <v>Tássia Castelli</v>
       </c>
-      <c r="E19" s="16" t="s">
-        <v>4</v>
+      <c r="E19" s="13" t="s">
+        <v>81</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="14" t="s">
@@ -4292,7 +4292,7 @@
       <c r="F21" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="G21" s="14" t="s">
         <v>38</v>
       </c>
       <c r="H21" s="4"/>
@@ -4322,7 +4322,7 @@
       <c r="F22" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="G22" s="6" t="s">
+      <c r="G22" s="14" t="s">
         <v>38</v>
       </c>
       <c r="H22" s="4"/>
@@ -4760,7 +4760,7 @@
       <c r="F36" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="G36" s="6" t="s">
+      <c r="G36" s="14" t="s">
         <v>38</v>
       </c>
       <c r="H36" s="4"/>
@@ -5188,7 +5188,7 @@
       <c r="F50" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="G50" s="6" t="s">
+      <c r="G50" s="14" t="s">
         <v>38</v>
       </c>
       <c r="H50" s="4"/>
@@ -5510,8 +5510,8 @@
   <dimension ref="A1:K58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="E31" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G57" sqref="G57"/>
+      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6165,7 +6165,7 @@
       <c r="F21" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="G21" s="14" t="s">
         <v>38</v>
       </c>
       <c r="H21" s="4"/>
@@ -6985,7 +6985,7 @@
       <c r="F48" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="G48" s="6" t="s">
+      <c r="G48" s="14" t="s">
         <v>38</v>
       </c>
       <c r="H48" s="4"/>
@@ -7257,7 +7257,7 @@
       <c r="F57" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="G57" s="14" t="s">
+      <c r="G57" s="6" t="s">
         <v>26</v>
       </c>
       <c r="H57" s="4" t="s">

</xml_diff>